<commit_message>
update result for gorilla/mux
</commit_message>
<xml_diff>
--- a/doc/which_is_the_fastest.xlsx
+++ b/doc/which_is_the_fastest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taicsuzu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taicsuzu/Documents/workspace/hobby/crystal/which_is_the_fastest/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Rails</t>
     <phoneticPr fontId="1"/>
@@ -54,6 +54,10 @@
   </si>
   <si>
     <t>Roda</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mux</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -175,7 +179,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -183,7 +187,7 @@
               <a:t>Ruby(</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -191,7 +195,7 @@
               <a:t>Rails</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -202,7 +206,7 @@
               <a:t>,</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0">
+              <a:rPr lang="en-US" sz="1600" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -213,7 +217,7 @@
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
@@ -221,7 +225,7 @@
               <a:t>Sinatra </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -229,7 +233,7 @@
               <a:t>and</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
@@ -237,7 +241,7 @@
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:srgbClr val="7030A0"/>
                 </a:solidFill>
@@ -245,11 +249,11 @@
               <a:t>Roda</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>) vs Crystal(</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
@@ -257,11 +261,11 @@
               <a:t>Kemal</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t> and </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1600">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
                 </a:solidFill>
@@ -269,26 +273,26 @@
               <a:t>route.cr</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>) vs</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
               <a:t> Go(</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0">
+              <a:rPr lang="en-US" sz="1600" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Echo</a:t>
+              <a:t>Echo and mux</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
               <a:t>)</a:t>
             </a:r>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="ja-JP" sz="1600"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1031,6 +1035,109 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>mux</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ja-JP"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.156</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.423</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
@@ -1042,11 +1149,11 @@
         </c:dLbls>
         <c:gapWidth val="164"/>
         <c:overlap val="-35"/>
-        <c:axId val="-2096307040"/>
-        <c:axId val="-2096303568"/>
+        <c:axId val="-2085929184"/>
+        <c:axId val="-2082284592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096307040"/>
+        <c:axId val="-2085929184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,7 +1190,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096303568"/>
+        <c:crossAx val="-2082284592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1091,7 +1198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096303568"/>
+        <c:axId val="-2082284592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1235,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096307040"/>
+        <c:crossAx val="-2085929184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1744,14 +1851,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>993595</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>69634</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>189950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>292495</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>68434</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>188750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2279,10 +2386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -2425,6 +2532,26 @@
       </c>
       <c r="G7">
         <v>5.8719999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.958</v>
+      </c>
+      <c r="E8">
+        <v>3.032</v>
+      </c>
+      <c r="F8">
+        <v>4.1559999999999997</v>
+      </c>
+      <c r="G8">
+        <v>5.423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>